<commit_message>
added a column for division_abbr
</commit_message>
<xml_diff>
--- a/docassemble/VTSharedYMLFile/data/sources/courts_list.xlsx
+++ b/docassemble/VTSharedYMLFile/data/sources/courts_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miabonardi/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksurette\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE7CE2C-E5E2-C541-A927-DC623C8D6ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDE5763-3A24-49FF-B953-5B284A07B896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6900" yWindow="1120" windowWidth="29040" windowHeight="15840" xr2:uid="{F13D4BD2-1651-4B43-8F6C-36F85B10F0AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F13D4BD2-1651-4B43-8F6C-36F85B10F0AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="97">
   <si>
     <t>name</t>
   </si>
@@ -321,6 +321,12 @@
   </si>
   <si>
     <t>arbitrary_attribute</t>
+  </si>
+  <si>
+    <t>division_abbr</t>
+  </si>
+  <si>
+    <t>Family</t>
   </si>
 </sst>
 </file>
@@ -427,9 +433,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -467,7 +473,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -573,7 +579,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -715,7 +721,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -723,33 +729,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A491E8-E2DE-9A4E-A3B9-C224836C99FE}">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="7" max="7" width="4.1640625" customWidth="1"/>
-    <col min="8" max="8" width="36.1640625" customWidth="1"/>
-    <col min="9" max="9" width="31.6640625" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="14.83203125" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" customWidth="1"/>
-    <col min="15" max="15" width="29.1640625" customWidth="1"/>
-    <col min="16" max="16" width="20.83203125" customWidth="1"/>
-    <col min="17" max="17" width="17.6640625" customWidth="1"/>
-    <col min="18" max="18" width="16.83203125" customWidth="1"/>
-    <col min="19" max="19" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.875" customWidth="1"/>
+    <col min="2" max="2" width="7.125" customWidth="1"/>
+    <col min="4" max="5" width="15" customWidth="1"/>
+    <col min="8" max="8" width="4.125" customWidth="1"/>
+    <col min="9" max="9" width="36.125" customWidth="1"/>
+    <col min="10" max="10" width="31.625" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="13" max="13" width="14.875" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="15.375" customWidth="1"/>
+    <col min="16" max="16" width="29.125" customWidth="1"/>
+    <col min="17" max="17" width="20.875" customWidth="1"/>
+    <col min="18" max="18" width="17.625" customWidth="1"/>
+    <col min="19" max="19" width="16.875" customWidth="1"/>
+    <col min="20" max="20" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -763,52 +769,55 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -818,38 +827,41 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" t="s">
         <v>44</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>58</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="5">
+      <c r="N2" s="5">
         <v>5753</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>20</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>44.013869999999997</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>-73.162989999999994</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -859,38 +871,41 @@
       <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>59</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>77</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="6">
+      <c r="N3" s="6">
         <v>5201</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>24</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>42.888089999999998</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>-73.198170000000005</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -900,41 +915,44 @@
       <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" t="s">
         <v>46</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>60</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>81</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>78</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>73</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="6">
+      <c r="N4" s="6">
         <v>5819</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>33</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>44.417960000000001</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>-72.020300000000006</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -944,41 +962,44 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" t="s">
         <v>47</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>61</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>82</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>79</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>74</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="6">
+      <c r="N5" s="6">
         <v>5401</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>34</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>44.47945</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>-73.217330000000004</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -988,35 +1009,38 @@
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" t="s">
         <v>48</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>60</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>93</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>25</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="6">
+      <c r="N6" s="6">
         <v>5905</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>35</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>92</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1026,32 +1050,35 @@
       <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" t="s">
         <v>49</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>62</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>83</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>26</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="6">
+      <c r="N7" s="6">
         <v>5478</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>36</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -1061,35 +1088,38 @@
       <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" t="s">
         <v>50</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>62</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>84</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>27</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="6">
+      <c r="N8" s="6">
         <v>5474</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>37</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>92</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1099,35 +1129,38 @@
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" t="s">
         <v>51</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>63</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>85</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>28</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="6">
+      <c r="N9" s="6">
         <v>5655</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>38</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>92</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1137,32 +1170,35 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" t="s">
         <v>52</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>64</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>86</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>29</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="6">
+      <c r="N10" s="6">
         <v>5038</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>39</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1172,35 +1208,38 @@
       <c r="D11" t="s">
         <v>18</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" t="s">
         <v>53</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>65</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>87</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>78</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>75</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="6">
+      <c r="N11" s="6">
         <v>5855</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>40</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1210,32 +1249,35 @@
       <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" t="s">
         <v>54</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>66</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>88</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>30</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="6">
+      <c r="N12" s="6">
         <v>5701</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>30</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1245,35 +1287,38 @@
       <c r="D13" t="s">
         <v>18</v>
       </c>
-      <c r="F13" t="s">
+      <c r="E13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" t="s">
         <v>55</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>67</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>89</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>78</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>31</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="6">
+      <c r="N13" s="6">
         <v>5641</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>41</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1283,35 +1328,38 @@
       <c r="D14" t="s">
         <v>18</v>
       </c>
-      <c r="F14" t="s">
+      <c r="E14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" t="s">
         <v>56</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>68</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>90</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>80</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>76</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="6">
+      <c r="N14" s="6">
         <v>5301</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>42</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1321,28 +1369,31 @@
       <c r="D15" t="s">
         <v>18</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" t="s">
         <v>57</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>69</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>91</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>32</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="6">
+      <c r="N15" s="6">
         <v>5001</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>43</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated to courts new email addresses on the courts list
</commit_message>
<xml_diff>
--- a/docassemble/VTSharedYMLFile/data/sources/courts_list.xlsx
+++ b/docassemble/VTSharedYMLFile/data/sources/courts_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksurette\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtlegalaid-my.sharepoint.com/personal/ksurette_lawlinevt_org/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDE5763-3A24-49FF-B953-5B284A07B896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{CF2E742D-44F9-4086-A5A6-A69C6F7ADFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36400547-8786-4530-91D1-7F050F48CF02}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F13D4BD2-1651-4B43-8F6C-36F85B10F0AA}"/>
   </bookViews>
@@ -212,42 +212,6 @@
     <t>802-295-8865</t>
   </si>
   <si>
-    <t>JUD.AddisonUnit@vermont.gov</t>
-  </si>
-  <si>
-    <t>JUD.BenningtonUnit@vermont.gov</t>
-  </si>
-  <si>
-    <t>JUD.CaledoniaEssexUnit@vermont.gov</t>
-  </si>
-  <si>
-    <t>JUD.ChittendenUnit@vermont.gov</t>
-  </si>
-  <si>
-    <t>JUD.FranklinGrandIsleunit@vermont.gov</t>
-  </si>
-  <si>
-    <t>JUD.LamoilleUnit@vermont.gov</t>
-  </si>
-  <si>
-    <t>JUD.OrangeUnit@vermont.gov</t>
-  </si>
-  <si>
-    <t>JUD.OrleansUnit@vermont.gov</t>
-  </si>
-  <si>
-    <t>JUD.RutlandUnit@vermont.gov</t>
-  </si>
-  <si>
-    <t>JUD.WashingtonUnit@vermont.gov</t>
-  </si>
-  <si>
-    <t>JUD.WindhamUnit@vermont.gov</t>
-  </si>
-  <si>
-    <t>JUD.WindsorUnit@vermont.gov</t>
-  </si>
-  <si>
     <t>PO Box 75, Guildhall, VT 05905</t>
   </si>
   <si>
@@ -327,6 +291,42 @@
   </si>
   <si>
     <t>Family</t>
+  </si>
+  <si>
+    <t>BenningtonUnit@vtcourts.gov</t>
+  </si>
+  <si>
+    <t>CaledoniaEssexUnit@vtcourts.gov</t>
+  </si>
+  <si>
+    <t>ChittendenUnit@vtcourts.gov</t>
+  </si>
+  <si>
+    <t>FranklinGrandIsleunit@vtcourts.gov</t>
+  </si>
+  <si>
+    <t>LamoilleUnit@vtcourts.gov</t>
+  </si>
+  <si>
+    <t>OrangeUnit@vtcourts.gov</t>
+  </si>
+  <si>
+    <t>OrleansUnit@vtcourts.gov</t>
+  </si>
+  <si>
+    <t>RutlandUnit@vtcourts.gov</t>
+  </si>
+  <si>
+    <t>WashingtonUnit@vtcourts.gov</t>
+  </si>
+  <si>
+    <t>WindhamUnit@vtcourts.gov</t>
+  </si>
+  <si>
+    <t>WindsorUnit@vtcourts.gov</t>
+  </si>
+  <si>
+    <t>AddisonUnit@vtcourts.gov</t>
   </si>
 </sst>
 </file>
@@ -336,7 +336,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -348,6 +348,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -400,10 +408,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -415,8 +424,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -732,7 +743,7 @@
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -769,7 +780,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -814,7 +825,7 @@
         <v>17</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -828,13 +839,13 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
         <v>44</v>
       </c>
-      <c r="I2" t="s">
-        <v>58</v>
+      <c r="I2" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="J2" t="s">
         <v>23</v>
@@ -858,7 +869,7 @@
         <v>-73.162989999999994</v>
       </c>
       <c r="S2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -872,16 +883,16 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G3" t="s">
         <v>45</v>
       </c>
-      <c r="I3" t="s">
-        <v>59</v>
+      <c r="I3" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="J3" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="L3" t="s">
         <v>24</v>
@@ -902,7 +913,7 @@
         <v>-73.198170000000005</v>
       </c>
       <c r="S3" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -916,22 +927,22 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G4" t="s">
         <v>46</v>
       </c>
-      <c r="I4" t="s">
-        <v>60</v>
+      <c r="I4" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="J4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="K4" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="L4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="M4" t="s">
         <v>22</v>
@@ -949,7 +960,7 @@
         <v>-72.020300000000006</v>
       </c>
       <c r="S4" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -963,22 +974,22 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G5" t="s">
         <v>47</v>
       </c>
-      <c r="I5" t="s">
-        <v>61</v>
+      <c r="I5" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="J5" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="L5" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="M5" t="s">
         <v>22</v>
@@ -996,7 +1007,7 @@
         <v>-73.217330000000004</v>
       </c>
       <c r="S5" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1010,16 +1021,16 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G6" t="s">
         <v>48</v>
       </c>
-      <c r="I6" t="s">
-        <v>60</v>
+      <c r="I6" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="J6" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="L6" t="s">
         <v>25</v>
@@ -1034,10 +1045,10 @@
         <v>35</v>
       </c>
       <c r="S6" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="T6" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1051,16 +1062,16 @@
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G7" t="s">
         <v>49</v>
       </c>
-      <c r="I7" t="s">
-        <v>62</v>
+      <c r="I7" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="J7" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="L7" t="s">
         <v>26</v>
@@ -1075,7 +1086,7 @@
         <v>36</v>
       </c>
       <c r="S7" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1089,16 +1100,16 @@
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G8" t="s">
         <v>50</v>
       </c>
-      <c r="I8" t="s">
-        <v>62</v>
+      <c r="I8" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="J8" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="L8" t="s">
         <v>27</v>
@@ -1113,10 +1124,10 @@
         <v>37</v>
       </c>
       <c r="S8" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="T8" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -1130,16 +1141,16 @@
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G9" t="s">
         <v>51</v>
       </c>
-      <c r="I9" t="s">
-        <v>63</v>
+      <c r="I9" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="J9" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="L9" t="s">
         <v>28</v>
@@ -1154,10 +1165,10 @@
         <v>38</v>
       </c>
       <c r="S9" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="T9" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -1171,16 +1182,16 @@
         <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G10" t="s">
         <v>52</v>
       </c>
-      <c r="I10" t="s">
-        <v>64</v>
+      <c r="I10" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="J10" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="L10" t="s">
         <v>29</v>
@@ -1195,7 +1206,7 @@
         <v>39</v>
       </c>
       <c r="S10" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1209,22 +1220,22 @@
         <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G11" t="s">
         <v>53</v>
       </c>
-      <c r="I11" t="s">
-        <v>65</v>
+      <c r="I11" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="J11" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="K11" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="L11" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="M11" t="s">
         <v>22</v>
@@ -1236,7 +1247,7 @@
         <v>40</v>
       </c>
       <c r="S11" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -1250,16 +1261,16 @@
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G12" t="s">
         <v>54</v>
       </c>
-      <c r="I12" t="s">
-        <v>66</v>
+      <c r="I12" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="J12" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="L12" t="s">
         <v>30</v>
@@ -1274,7 +1285,7 @@
         <v>30</v>
       </c>
       <c r="S12" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -1288,19 +1299,19 @@
         <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G13" t="s">
         <v>55</v>
       </c>
-      <c r="I13" t="s">
-        <v>67</v>
+      <c r="I13" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="J13" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="K13" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="L13" t="s">
         <v>31</v>
@@ -1315,7 +1326,7 @@
         <v>41</v>
       </c>
       <c r="S13" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1329,22 +1340,22 @@
         <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G14" t="s">
         <v>56</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J14" t="s">
+        <v>78</v>
+      </c>
+      <c r="K14" t="s">
         <v>68</v>
       </c>
-      <c r="J14" t="s">
-        <v>90</v>
-      </c>
-      <c r="K14" t="s">
-        <v>80</v>
-      </c>
       <c r="L14" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="M14" t="s">
         <v>22</v>
@@ -1356,7 +1367,7 @@
         <v>42</v>
       </c>
       <c r="S14" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -1370,16 +1381,16 @@
         <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G15" t="s">
         <v>57</v>
       </c>
-      <c r="I15" t="s">
-        <v>69</v>
+      <c r="I15" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="J15" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="L15" t="s">
         <v>32</v>
@@ -1394,11 +1405,27 @@
         <v>43</v>
       </c>
       <c r="S15" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" display="AddisonUnit@vermont.gov" xr:uid="{CE067579-4D2A-4FB7-BC20-71CF63E84A64}"/>
+    <hyperlink ref="I3" r:id="rId2" display="BenningtonUnit@vermont.gov" xr:uid="{FB72F267-E788-4851-A3D1-CA77ACFF585C}"/>
+    <hyperlink ref="I4" r:id="rId3" display="CaledoniaEssexUnit@vermont.gov" xr:uid="{1A175C18-6B0E-45DA-900D-8291E2C78C99}"/>
+    <hyperlink ref="I5" r:id="rId4" display="ChittendenUnit@vermont.gov" xr:uid="{9FF34C42-4441-46C0-BE1D-9155E2E8825B}"/>
+    <hyperlink ref="I6" r:id="rId5" display="CaledoniaEssexUnit@vermont.gov" xr:uid="{760AAC80-1B97-436E-AEB1-09E75778AC9D}"/>
+    <hyperlink ref="I7" r:id="rId6" display="FranklinGrandIsleunit@vermont.gov" xr:uid="{8F842D91-7453-45BA-A54E-CBCE4FE0577D}"/>
+    <hyperlink ref="I8" r:id="rId7" display="FranklinGrandIsleunit@vermont.gov" xr:uid="{7871886E-3C12-4CEC-B5B2-18622AD5509B}"/>
+    <hyperlink ref="I9" r:id="rId8" display="LamoilleUnit@vermont.gov" xr:uid="{69019928-95E2-41A0-9CD5-BDA65F0890D7}"/>
+    <hyperlink ref="I10" r:id="rId9" display="OrangeUnit@vermont.gov" xr:uid="{E536316C-27C7-4716-B9B2-FF9CE5C9D428}"/>
+    <hyperlink ref="I11" r:id="rId10" display="OrleansUnit@vermont.gov" xr:uid="{2F4F8B7F-2002-495A-A50F-5BC3EA27B661}"/>
+    <hyperlink ref="I12" r:id="rId11" display="RutlandUnit@vermont.gov" xr:uid="{E84206E9-32FD-488A-9404-A74109553EE1}"/>
+    <hyperlink ref="I13" r:id="rId12" display="WashingtonUnit@vermont.gov" xr:uid="{62688A28-3730-46D9-8F5B-6CB580AB3A11}"/>
+    <hyperlink ref="I14" r:id="rId13" display="WindhamUnit@vermont.gov" xr:uid="{AE616A9A-A9CF-473C-AA71-EF580C860226}"/>
+    <hyperlink ref="I15" r:id="rId14" display="WindsorUnit@vermont.gov" xr:uid="{79E27C0A-1083-4C5E-B394-01C1BC9FC0CD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated the courts list spreadsheet with more VT courts
</commit_message>
<xml_diff>
--- a/docassemble/VTSharedYMLFile/data/sources/courts_list.xlsx
+++ b/docassemble/VTSharedYMLFile/data/sources/courts_list.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtlegalaid-my.sharepoint.com/personal/ksurette_lawlinevt_org/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtlegalaid-my.sharepoint.com/personal/ksurette_lawlinevt_org/Documents/TIG 22/Docassemble guided interviews Suffolk project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{CF2E742D-44F9-4086-A5A6-A69C6F7ADFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36400547-8786-4530-91D1-7F050F48CF02}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{BED62D44-0F95-49D0-9C24-2C44B691692B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60980042-C126-4FFF-913E-803E2610E9F4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F13D4BD2-1651-4B43-8F6C-36F85B10F0AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="132">
   <si>
     <t>name</t>
   </si>
@@ -327,6 +327,111 @@
   </si>
   <si>
     <t>AddisonUnit@vtcourts.gov</t>
+  </si>
+  <si>
+    <t>Civil Division</t>
+  </si>
+  <si>
+    <t>Civil</t>
+  </si>
+  <si>
+    <t>207 South Street</t>
+  </si>
+  <si>
+    <t>802-447-2700</t>
+  </si>
+  <si>
+    <t>civil court</t>
+  </si>
+  <si>
+    <t>802-863-3467</t>
+  </si>
+  <si>
+    <t>175 Main Street</t>
+  </si>
+  <si>
+    <t>PO Box 187, Burlington, VT 05402</t>
+  </si>
+  <si>
+    <t>802-524-7993</t>
+  </si>
+  <si>
+    <t>17 Church Street</t>
+  </si>
+  <si>
+    <t>802-775-4394</t>
+  </si>
+  <si>
+    <t>83 Center Street</t>
+  </si>
+  <si>
+    <t>802-828-2091</t>
+  </si>
+  <si>
+    <t>65 State Street</t>
+  </si>
+  <si>
+    <t>Montpelier</t>
+  </si>
+  <si>
+    <t>802-365-7979</t>
+  </si>
+  <si>
+    <t>7 Court Street</t>
+  </si>
+  <si>
+    <t>Newfane</t>
+  </si>
+  <si>
+    <t>PO Box 207, Newfane, VT 05345</t>
+  </si>
+  <si>
+    <t>802-457-2121</t>
+  </si>
+  <si>
+    <t>12 The Green</t>
+  </si>
+  <si>
+    <t>Woodstock</t>
+  </si>
+  <si>
+    <t>Probate</t>
+  </si>
+  <si>
+    <t>Probate Division</t>
+  </si>
+  <si>
+    <t>probate court</t>
+  </si>
+  <si>
+    <t>802-651-1518</t>
+  </si>
+  <si>
+    <t>802-524-4112</t>
+  </si>
+  <si>
+    <t>802-775-0114</t>
+  </si>
+  <si>
+    <t>Environmental Division</t>
+  </si>
+  <si>
+    <t>Environmental</t>
+  </si>
+  <si>
+    <t>802-951-1740</t>
+  </si>
+  <si>
+    <t>EnvironmentalDivision@vtcourts.gov</t>
+  </si>
+  <si>
+    <t>2nd Floor, Suite 303</t>
+  </si>
+  <si>
+    <t>environmental court</t>
+  </si>
+  <si>
+    <t>Statewide</t>
   </si>
 </sst>
 </file>
@@ -441,6 +546,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -740,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A491E8-E2DE-9A4E-A3B9-C224836C99FE}">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -751,6 +860,8 @@
     <col min="1" max="1" width="23.875" customWidth="1"/>
     <col min="2" max="2" width="7.125" customWidth="1"/>
     <col min="4" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="7.125" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="4.125" customWidth="1"/>
     <col min="9" max="9" width="36.125" customWidth="1"/>
     <col min="10" max="10" width="31.625" customWidth="1"/>
@@ -957,6 +1068,7 @@
         <v>44.417960000000001</v>
       </c>
       <c r="R4">
+        <f>R18</f>
         <v>-72.020300000000006</v>
       </c>
       <c r="S4" t="s">
@@ -1406,6 +1518,1172 @@
       </c>
       <c r="S15" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J16" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="5">
+        <v>5753</v>
+      </c>
+      <c r="O16" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q16">
+        <v>44.013869999999997</v>
+      </c>
+      <c r="R16">
+        <v>-73.162989999999994</v>
+      </c>
+      <c r="S16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J17" t="s">
+        <v>99</v>
+      </c>
+      <c r="L17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="6">
+        <v>5201</v>
+      </c>
+      <c r="O17" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q17">
+        <v>42.888089999999998</v>
+      </c>
+      <c r="R17">
+        <v>-73.198170000000005</v>
+      </c>
+      <c r="S17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J18" t="s">
+        <v>69</v>
+      </c>
+      <c r="K18" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" t="s">
+        <v>61</v>
+      </c>
+      <c r="M18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="6">
+        <v>5819</v>
+      </c>
+      <c r="O18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q18">
+        <v>44.417960000000001</v>
+      </c>
+      <c r="R18">
+        <f>R32</f>
+        <v>-72.020300000000006</v>
+      </c>
+      <c r="S18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" t="s">
+        <v>102</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" t="s">
+        <v>103</v>
+      </c>
+      <c r="L19" t="s">
+        <v>62</v>
+      </c>
+      <c r="M19" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="6">
+        <v>5402</v>
+      </c>
+      <c r="O19" t="s">
+        <v>34</v>
+      </c>
+      <c r="S19" t="s">
+        <v>101</v>
+      </c>
+      <c r="T19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J20" t="s">
+        <v>81</v>
+      </c>
+      <c r="L20" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="6">
+        <v>5905</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="S20" t="s">
+        <v>101</v>
+      </c>
+      <c r="T20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" t="s">
+        <v>105</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J21" t="s">
+        <v>106</v>
+      </c>
+      <c r="L21" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="6">
+        <v>5478</v>
+      </c>
+      <c r="O21" t="s">
+        <v>36</v>
+      </c>
+      <c r="S21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" t="s">
+        <v>50</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J22" t="s">
+        <v>72</v>
+      </c>
+      <c r="L22" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" s="6">
+        <v>5474</v>
+      </c>
+      <c r="O22" t="s">
+        <v>37</v>
+      </c>
+      <c r="S22" t="s">
+        <v>101</v>
+      </c>
+      <c r="T22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" t="s">
+        <v>51</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="J23" t="s">
+        <v>73</v>
+      </c>
+      <c r="L23" t="s">
+        <v>28</v>
+      </c>
+      <c r="M23" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="6">
+        <v>5655</v>
+      </c>
+      <c r="O23" t="s">
+        <v>38</v>
+      </c>
+      <c r="S23" t="s">
+        <v>101</v>
+      </c>
+      <c r="T23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G24" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" t="s">
+        <v>74</v>
+      </c>
+      <c r="L24" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24" s="6">
+        <v>5038</v>
+      </c>
+      <c r="O24" t="s">
+        <v>39</v>
+      </c>
+      <c r="S24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J25" t="s">
+        <v>75</v>
+      </c>
+      <c r="L25" t="s">
+        <v>63</v>
+      </c>
+      <c r="M25" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" s="6">
+        <v>5855</v>
+      </c>
+      <c r="O25" t="s">
+        <v>40</v>
+      </c>
+      <c r="S25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J26" t="s">
+        <v>108</v>
+      </c>
+      <c r="L26" t="s">
+        <v>30</v>
+      </c>
+      <c r="M26" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26" s="6">
+        <v>5701</v>
+      </c>
+      <c r="O26" t="s">
+        <v>30</v>
+      </c>
+      <c r="S26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" t="s">
+        <v>98</v>
+      </c>
+      <c r="G27" t="s">
+        <v>109</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="J27" t="s">
+        <v>110</v>
+      </c>
+      <c r="L27" t="s">
+        <v>111</v>
+      </c>
+      <c r="M27" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27" s="6">
+        <v>5602</v>
+      </c>
+      <c r="O27" t="s">
+        <v>41</v>
+      </c>
+      <c r="S27" t="s">
+        <v>101</v>
+      </c>
+      <c r="T27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" t="s">
+        <v>112</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J28" t="s">
+        <v>113</v>
+      </c>
+      <c r="L28" t="s">
+        <v>114</v>
+      </c>
+      <c r="M28" t="s">
+        <v>22</v>
+      </c>
+      <c r="N28" s="6">
+        <v>5345</v>
+      </c>
+      <c r="O28" t="s">
+        <v>42</v>
+      </c>
+      <c r="S28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" t="s">
+        <v>116</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J29" t="s">
+        <v>117</v>
+      </c>
+      <c r="L29" t="s">
+        <v>118</v>
+      </c>
+      <c r="M29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29" s="6">
+        <v>5091</v>
+      </c>
+      <c r="O29" t="s">
+        <v>43</v>
+      </c>
+      <c r="S29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" t="s">
+        <v>119</v>
+      </c>
+      <c r="G30" t="s">
+        <v>44</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J30" t="s">
+        <v>23</v>
+      </c>
+      <c r="L30" t="s">
+        <v>21</v>
+      </c>
+      <c r="M30" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30" s="6">
+        <v>5753</v>
+      </c>
+      <c r="O30" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q30">
+        <v>44.013869999999997</v>
+      </c>
+      <c r="R30">
+        <v>-73.162989999999994</v>
+      </c>
+      <c r="S30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" t="s">
+        <v>119</v>
+      </c>
+      <c r="G31" t="s">
+        <v>100</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J31" t="s">
+        <v>99</v>
+      </c>
+      <c r="L31" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" s="6">
+        <v>5201</v>
+      </c>
+      <c r="O31" t="s">
+        <v>24</v>
+      </c>
+      <c r="S31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" t="s">
+        <v>119</v>
+      </c>
+      <c r="G32" t="s">
+        <v>46</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J32" t="s">
+        <v>69</v>
+      </c>
+      <c r="L32" t="s">
+        <v>61</v>
+      </c>
+      <c r="M32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N32" s="6">
+        <v>5819</v>
+      </c>
+      <c r="O32" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q32">
+        <v>44.417960000000001</v>
+      </c>
+      <c r="R32">
+        <v>-72.020300000000006</v>
+      </c>
+      <c r="S32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E33" t="s">
+        <v>119</v>
+      </c>
+      <c r="G33" t="s">
+        <v>122</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="J33" t="s">
+        <v>103</v>
+      </c>
+      <c r="L33" t="s">
+        <v>62</v>
+      </c>
+      <c r="M33" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" s="6">
+        <v>5401</v>
+      </c>
+      <c r="O33" t="s">
+        <v>34</v>
+      </c>
+      <c r="S33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>120</v>
+      </c>
+      <c r="E34" t="s">
+        <v>119</v>
+      </c>
+      <c r="G34" t="s">
+        <v>48</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J34" t="s">
+        <v>81</v>
+      </c>
+      <c r="L34" t="s">
+        <v>25</v>
+      </c>
+      <c r="M34" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34" s="6">
+        <v>5905</v>
+      </c>
+      <c r="O34" t="s">
+        <v>35</v>
+      </c>
+      <c r="S34" t="s">
+        <v>121</v>
+      </c>
+      <c r="T34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" t="s">
+        <v>120</v>
+      </c>
+      <c r="E35" t="s">
+        <v>119</v>
+      </c>
+      <c r="G35" t="s">
+        <v>123</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J35" t="s">
+        <v>106</v>
+      </c>
+      <c r="L35" t="s">
+        <v>26</v>
+      </c>
+      <c r="M35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35" s="6">
+        <v>5478</v>
+      </c>
+      <c r="O35" t="s">
+        <v>36</v>
+      </c>
+      <c r="S35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
+        <v>120</v>
+      </c>
+      <c r="E36" t="s">
+        <v>119</v>
+      </c>
+      <c r="G36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J36" t="s">
+        <v>72</v>
+      </c>
+      <c r="L36" t="s">
+        <v>27</v>
+      </c>
+      <c r="M36" t="s">
+        <v>22</v>
+      </c>
+      <c r="N36" s="6">
+        <v>5474</v>
+      </c>
+      <c r="O36" t="s">
+        <v>37</v>
+      </c>
+      <c r="S36" t="s">
+        <v>121</v>
+      </c>
+      <c r="T36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
+        <v>120</v>
+      </c>
+      <c r="E37" t="s">
+        <v>119</v>
+      </c>
+      <c r="G37" t="s">
+        <v>51</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="J37" t="s">
+        <v>73</v>
+      </c>
+      <c r="L37" t="s">
+        <v>28</v>
+      </c>
+      <c r="M37" t="s">
+        <v>22</v>
+      </c>
+      <c r="N37" s="6">
+        <v>5655</v>
+      </c>
+      <c r="O37" t="s">
+        <v>38</v>
+      </c>
+      <c r="S37" t="s">
+        <v>121</v>
+      </c>
+      <c r="T37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" t="s">
+        <v>120</v>
+      </c>
+      <c r="E38" t="s">
+        <v>119</v>
+      </c>
+      <c r="G38" t="s">
+        <v>52</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J38" t="s">
+        <v>74</v>
+      </c>
+      <c r="L38" t="s">
+        <v>29</v>
+      </c>
+      <c r="M38" t="s">
+        <v>22</v>
+      </c>
+      <c r="N38" s="6">
+        <v>5038</v>
+      </c>
+      <c r="O38" t="s">
+        <v>39</v>
+      </c>
+      <c r="S38" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" t="s">
+        <v>119</v>
+      </c>
+      <c r="G39" t="s">
+        <v>53</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J39" t="s">
+        <v>75</v>
+      </c>
+      <c r="L39" t="s">
+        <v>63</v>
+      </c>
+      <c r="M39" t="s">
+        <v>22</v>
+      </c>
+      <c r="N39" s="6">
+        <v>5855</v>
+      </c>
+      <c r="O39" t="s">
+        <v>40</v>
+      </c>
+      <c r="S39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" t="s">
+        <v>120</v>
+      </c>
+      <c r="E40" t="s">
+        <v>119</v>
+      </c>
+      <c r="G40" t="s">
+        <v>124</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J40" t="s">
+        <v>108</v>
+      </c>
+      <c r="L40" t="s">
+        <v>30</v>
+      </c>
+      <c r="M40" t="s">
+        <v>22</v>
+      </c>
+      <c r="N40" s="6">
+        <v>5701</v>
+      </c>
+      <c r="O40" t="s">
+        <v>30</v>
+      </c>
+      <c r="S40" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" t="s">
+        <v>120</v>
+      </c>
+      <c r="E41" t="s">
+        <v>119</v>
+      </c>
+      <c r="G41" t="s">
+        <v>109</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="J41" t="s">
+        <v>110</v>
+      </c>
+      <c r="L41" t="s">
+        <v>111</v>
+      </c>
+      <c r="M41" t="s">
+        <v>22</v>
+      </c>
+      <c r="N41" s="6">
+        <v>5602</v>
+      </c>
+      <c r="O41" t="s">
+        <v>41</v>
+      </c>
+      <c r="S41" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" t="s">
+        <v>120</v>
+      </c>
+      <c r="E42" t="s">
+        <v>119</v>
+      </c>
+      <c r="G42" t="s">
+        <v>56</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J42" t="s">
+        <v>78</v>
+      </c>
+      <c r="K42" t="s">
+        <v>68</v>
+      </c>
+      <c r="L42" t="s">
+        <v>64</v>
+      </c>
+      <c r="M42" t="s">
+        <v>22</v>
+      </c>
+      <c r="N42" s="6">
+        <v>5301</v>
+      </c>
+      <c r="O42" t="s">
+        <v>42</v>
+      </c>
+      <c r="S42" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" t="s">
+        <v>120</v>
+      </c>
+      <c r="E43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G43" t="s">
+        <v>116</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J43" t="s">
+        <v>117</v>
+      </c>
+      <c r="L43" t="s">
+        <v>118</v>
+      </c>
+      <c r="M43" t="s">
+        <v>22</v>
+      </c>
+      <c r="N43" s="6">
+        <v>5091</v>
+      </c>
+      <c r="O43" t="s">
+        <v>43</v>
+      </c>
+      <c r="S43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" t="s">
+        <v>125</v>
+      </c>
+      <c r="E44" t="s">
+        <v>126</v>
+      </c>
+      <c r="G44" t="s">
+        <v>127</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="J44" t="s">
+        <v>70</v>
+      </c>
+      <c r="K44" t="s">
+        <v>129</v>
+      </c>
+      <c r="L44" t="s">
+        <v>62</v>
+      </c>
+      <c r="M44" t="s">
+        <v>22</v>
+      </c>
+      <c r="N44" s="6">
+        <v>5401</v>
+      </c>
+      <c r="O44" t="s">
+        <v>34</v>
+      </c>
+      <c r="S44" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1424,8 +2702,37 @@
     <hyperlink ref="I13" r:id="rId12" display="WashingtonUnit@vermont.gov" xr:uid="{62688A28-3730-46D9-8F5B-6CB580AB3A11}"/>
     <hyperlink ref="I14" r:id="rId13" display="WindhamUnit@vermont.gov" xr:uid="{AE616A9A-A9CF-473C-AA71-EF580C860226}"/>
     <hyperlink ref="I15" r:id="rId14" display="WindsorUnit@vermont.gov" xr:uid="{79E27C0A-1083-4C5E-B394-01C1BC9FC0CD}"/>
+    <hyperlink ref="I16" r:id="rId15" display="AddisonUnit@vermont.gov" xr:uid="{4A55FA55-EEB3-4B06-8E9A-C83765B14581}"/>
+    <hyperlink ref="I17" r:id="rId16" display="BenningtonUnit@vermont.gov" xr:uid="{F5846B64-7D2B-4EA9-A752-DEAE4E72E362}"/>
+    <hyperlink ref="I18" r:id="rId17" xr:uid="{A4A4A874-E4B7-44B8-9E90-89BB39E96775}"/>
+    <hyperlink ref="I19" r:id="rId18" xr:uid="{6A202E57-4DE0-4D16-9F4E-7D8F65CE1762}"/>
+    <hyperlink ref="I20" r:id="rId19" xr:uid="{0682AAD8-00E5-4949-B772-70778872FFF5}"/>
+    <hyperlink ref="I21" r:id="rId20" xr:uid="{8712C140-D413-43C0-A867-011098A3B272}"/>
+    <hyperlink ref="I22" r:id="rId21" xr:uid="{0D34FD78-2607-4346-AB53-AE0B6D796361}"/>
+    <hyperlink ref="I23" r:id="rId22" xr:uid="{92B4C53D-7BE3-46A3-B6C5-C07526084989}"/>
+    <hyperlink ref="I24" r:id="rId23" xr:uid="{A0D36FC9-2BD1-4ECB-A278-753DCCF813BC}"/>
+    <hyperlink ref="I25" r:id="rId24" xr:uid="{1BD2A3C4-BA91-459E-B929-C77E984B3450}"/>
+    <hyperlink ref="I26" r:id="rId25" xr:uid="{E6D72075-6EB0-4F34-A194-C1F9AB8E8F1A}"/>
+    <hyperlink ref="I27" r:id="rId26" xr:uid="{8D40A5D5-B35C-4505-B035-5AAB4A44A1BC}"/>
+    <hyperlink ref="I28" r:id="rId27" xr:uid="{09EFE2F4-2821-4608-B0B0-E0137AA308CD}"/>
+    <hyperlink ref="I29" r:id="rId28" xr:uid="{16F6DBC8-C336-483E-B9EF-76F76D347A6E}"/>
+    <hyperlink ref="I30" r:id="rId29" xr:uid="{0F7B39CE-DD14-43F4-A959-891D6B4E1F34}"/>
+    <hyperlink ref="I31" r:id="rId30" xr:uid="{6FC579A3-819C-47E6-9A7B-C93CAC63E5A3}"/>
+    <hyperlink ref="I32" r:id="rId31" xr:uid="{219729DB-1039-4400-9B07-43C2C104D9AD}"/>
+    <hyperlink ref="I33" r:id="rId32" xr:uid="{91FEC728-C373-46FD-B76E-96B37C0C0D09}"/>
+    <hyperlink ref="I34" r:id="rId33" xr:uid="{0BD2AB8E-3278-4694-9E73-822BAF35073A}"/>
+    <hyperlink ref="I35" r:id="rId34" xr:uid="{84CDACA3-ED0A-405E-9804-C8BAA8E75337}"/>
+    <hyperlink ref="I36" r:id="rId35" xr:uid="{1C2DB7AC-F3AE-41C9-AE84-2D800F417D82}"/>
+    <hyperlink ref="I37" r:id="rId36" xr:uid="{FBB062B1-C0B9-4A98-BBF1-F36C43FAE49B}"/>
+    <hyperlink ref="I38" r:id="rId37" xr:uid="{3DD10C8C-E6FD-41DF-853D-D761505E635F}"/>
+    <hyperlink ref="I39" r:id="rId38" xr:uid="{C0AF86C7-025C-4CE2-8B11-7CE370813380}"/>
+    <hyperlink ref="I40" r:id="rId39" xr:uid="{44AE4776-9A02-47E7-A3A9-773B01319A55}"/>
+    <hyperlink ref="I41" r:id="rId40" xr:uid="{85A98D47-0F16-4024-BDA1-203C9C7F5EAD}"/>
+    <hyperlink ref="I42" r:id="rId41" xr:uid="{7985C3BF-D1EC-4776-9D55-DFDCFB4FD907}"/>
+    <hyperlink ref="I43" r:id="rId42" xr:uid="{887F9765-37FE-436D-AD0B-EFBB5DC9E16B}"/>
+    <hyperlink ref="I44" r:id="rId43" xr:uid="{9D15AA29-6BD6-40AD-BBD0-FA9004238297}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId44"/>
 </worksheet>
 </file>
</xml_diff>